<commit_message>
Update logique.js, questionnaire.js, and questionnaire.php
1. logique.js:
   - Add event listeners for 'nin_exploitant' and 'nom_exploitation' input
</commit_message>
<xml_diff>
--- a/test/Contrôles divers.xlsx
+++ b/test/Contrôles divers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Disque D\Mes documents\3- MADR\RGA\RGA 2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rga\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813A0D04-33B3-4E59-A3A2-2F37D8292107}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE264AED-4571-4328-8F28-82FBCA3F6B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{BDC3A8CC-940F-4C61-8C7E-5D3E0EF57969}"/>
+    <workbookView xWindow="-24120" yWindow="4275" windowWidth="24240" windowHeight="13020" xr2:uid="{BDC3A8CC-940F-4C61-8C7E-5D3E0EF57969}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -452,39 +452,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Volume (m</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>Type et nombre du matériel agricole ?</t>
   </si>
   <si>
@@ -848,12 +815,38 @@
   <si>
     <t xml:space="preserve">Remettre les options (Type d'assurance) à "" en cas de changement d'option (Avez vous contracté une assurance agricoles ?) de Oui à Non </t>
   </si>
+  <si>
+    <r>
+      <t>Volume (m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -893,13 +886,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF212529"/>
       <name val="Segoe UI"/>
       <family val="2"/>
@@ -925,12 +911,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -945,7 +943,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -956,23 +954,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -995,16 +1002,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>37637</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>94911</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>704387</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>256836</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1027,7 +1034,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11191875" y="12458700"/>
+          <a:off x="13382625" y="12811125"/>
           <a:ext cx="3704762" cy="2714286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1339,14 +1346,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CEBEDDF-FD66-40DD-88B1-FAA8A0C63C72}">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
-    <col min="2" max="2" width="44.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="60.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.28515625" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11.42578125" style="1"/>
@@ -1361,7 +1368,7 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1371,33 +1378,35 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
         <v>12</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
         <v>13</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>14</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1408,7 +1417,7 @@
       <c r="A6" s="1">
         <v>15</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1419,7 +1428,7 @@
       <c r="A7" s="1">
         <v>16</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1433,35 +1442,36 @@
       <c r="A8" s="1">
         <v>17</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="9" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
         <v>18</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
         <v>19</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1469,40 +1479,41 @@
       <c r="A11" s="1">
         <v>28</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="12" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
         <v>31</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="B12" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>32</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>87</v>
+      <c r="B13" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>34</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -1513,7 +1524,7 @@
       <c r="A15" s="1">
         <v>38</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -1524,7 +1535,7 @@
       <c r="A16" s="1">
         <v>42</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1535,7 +1546,7 @@
       <c r="A17" s="1">
         <v>43</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1549,7 +1560,7 @@
       <c r="A18" s="1">
         <v>44</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -1563,18 +1574,18 @@
       <c r="A19" s="1">
         <v>45</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>46</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -1585,7 +1596,7 @@
       <c r="A21" s="1">
         <v>51</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1596,7 +1607,7 @@
       <c r="A22" s="1">
         <v>54</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -1610,7 +1621,7 @@
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -1621,29 +1632,29 @@
       <c r="A24" s="1">
         <v>58</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>60</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>91</v>
+      <c r="B25" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>63</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="2" t="s">
         <v>45</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -1654,21 +1665,21 @@
       <c r="A27" s="1">
         <v>64</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>67</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -1679,7 +1690,7 @@
       <c r="A29" s="1">
         <v>69</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -1690,21 +1701,22 @@
       <c r="A30" s="1">
         <v>70</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+    <row r="31" spans="1:4" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="8">
         <v>72</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="C31" s="9"/>
+      <c r="D31" s="12" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1712,10 +1724,10 @@
       <c r="A32" s="1">
         <v>74</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="B32" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="9" t="s">
         <v>56</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -1726,10 +1738,10 @@
       <c r="A33" s="1">
         <v>75</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="B33" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>57</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -1740,10 +1752,10 @@
       <c r="A34" s="1">
         <v>76</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="B34" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>58</v>
       </c>
       <c r="D34" s="2" t="s">
@@ -1754,7 +1766,7 @@
       <c r="A35" s="1">
         <v>78</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="2" t="s">
         <v>60</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -1765,7 +1777,7 @@
       <c r="A36" s="1">
         <v>80</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -1776,7 +1788,7 @@
       <c r="A37" s="1">
         <v>82</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="2" t="s">
         <v>62</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -1787,7 +1799,7 @@
       <c r="A38" s="1">
         <v>84</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -1798,10 +1810,10 @@
       <c r="A39" s="1">
         <v>91</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C39" s="4" t="s">
+      <c r="B39" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="11" t="s">
         <v>68</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -1812,10 +1824,10 @@
       <c r="A40" s="1">
         <v>92</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C40" s="4" t="s">
+      <c r="B40" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="11" t="s">
         <v>68</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -1824,167 +1836,170 @@
     </row>
     <row r="41" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C41" s="4" t="s">
+      <c r="D41" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+    </row>
+    <row r="42" spans="1:4" s="8" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="8">
         <v>111</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>72</v>
-      </c>
+      <c r="C42" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" s="9"/>
     </row>
     <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>112</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>73</v>
+      <c r="B43" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>116</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>117</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>118</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>119</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D47" s="2" t="s">
+    </row>
+    <row r="48" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="8">
+        <v>121</v>
+      </c>
+      <c r="B48" s="9" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>121</v>
-      </c>
-      <c r="B48" s="5" t="s">
+      <c r="C48" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+      <c r="D48" s="9"/>
+    </row>
+    <row r="49" spans="1:4" s="8" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="8">
         <v>124</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>106</v>
-      </c>
+      <c r="D49" s="9"/>
     </row>
     <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>124</v>
       </c>
-      <c r="B50" s="7" t="s">
-        <v>103</v>
+      <c r="B50" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>126</v>
       </c>
-      <c r="B51" s="7" t="s">
-        <v>104</v>
+      <c r="B51" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>130</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D52" s="2" t="s">
+    </row>
+    <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" s="6" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
+      <c r="D53" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B53" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="D53" s="2" t="s">
+    </row>
+    <row r="54" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B54" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B54" s="5" t="s">
+      <c r="D54" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D54" s="2" t="s">
+    </row>
+    <row r="55" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B55" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B55" s="5" t="s">
+      <c r="D55" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>